<commit_message>
Add build configuration and Procfile for Heroku deployment
</commit_message>
<xml_diff>
--- a/src/main/resources/template/Estimate/clps001.xlsx
+++ b/src/main/resources/template/Estimate/clps001.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>作業内容</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -219,16 +219,7 @@
     <t>aa</t>
   </si>
   <si>
-    <t>2024-06-01 - 2024-08-31</t>
-  </si>
-  <si>
-    <t>2024-09-01 - 2024-11-30</t>
-  </si>
-  <si>
     <t>2024-12-01 - 2025-02-28</t>
-  </si>
-  <si>
-    <t>2025-03-01 - 2025-05-31</t>
   </si>
   <si>
     <t xml:space="preserve">　　　　担当者：u　　　　承認者：d</t>
@@ -472,7 +463,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,60 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1112,7 +1049,7 @@
     <row r="14" spans="2:8" s="9" customFormat="1">
       <c r="D14" s="10"/>
       <c r="F14" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -1169,7 +1106,7 @@
       </c>
       <c r="C21" s="25" t="n">
         <f>H33</f>
-        <v>5280000.0</v>
+        <v>1320000.0</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="12"/>
@@ -1232,66 +1169,30 @@
     </row>
     <row r="25" spans="2:8" s="9" customFormat="1" ht="35.1" customHeight="1">
       <c r="B25" s="24"/>
-      <c r="C25" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="44" t="n">
-        <v>400000.0</v>
-      </c>
-      <c r="G25" s="45" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H25" s="46" t="n">
-        <v>1200000.0</v>
-      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
     </row>
     <row r="26" spans="2:8" s="9" customFormat="1" ht="35.1" customHeight="1">
       <c r="B26" s="24"/>
-      <c r="C26" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="50" t="n">
-        <v>400000.0</v>
-      </c>
-      <c r="G26" s="51" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H26" s="52" t="n">
-        <v>1200000.0</v>
-      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
     </row>
     <row r="27" spans="2:8" s="9" customFormat="1" ht="35.1" customHeight="1">
       <c r="B27" s="24"/>
-      <c r="C27" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="56" t="n">
-        <v>400000.0</v>
-      </c>
-      <c r="G27" s="57" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H27" s="58" t="n">
-        <v>1200000.0</v>
-      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
     </row>
     <row r="28" spans="2:8" s="9" customFormat="1" ht="35.1" customHeight="1">
       <c r="B28" s="24"/>
@@ -1331,7 +1232,7 @@
       <c r="G31" s="34"/>
       <c r="H31" s="8" t="n">
         <f>SUM(H24:H30)</f>
-        <v>4800000.0</v>
+        <v>1200000.0</v>
       </c>
     </row>
     <row r="32" spans="2:8" s="9" customFormat="1" ht="35.1" customHeight="1">
@@ -1345,7 +1246,7 @@
       <c r="G32" s="34"/>
       <c r="H32" s="8" t="n">
         <f>H31*0.1</f>
-        <v>480000.0</v>
+        <v>120000.0</v>
       </c>
     </row>
     <row r="33" spans="2:8" s="9" customFormat="1" ht="35.1" customHeight="1">
@@ -1359,7 +1260,7 @@
       <c r="G33" s="34"/>
       <c r="H33" s="8" t="n">
         <f>SUM(H31:H32)</f>
-        <v>5280000.0</v>
+        <v>1320000.0</v>
       </c>
     </row>
     <row r="34" spans="2:8" s="9" customFormat="1">

</xml_diff>